<commit_message>
Committed from VS 2017
</commit_message>
<xml_diff>
--- a/EmailParser/bin/Debug/Output/OrderBook1.xlsx
+++ b/EmailParser/bin/Debug/Output/OrderBook1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bin.wu\source\repos\EmailParser\EmailParser\bin\Debug\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593520E0-7D11-4788-A4C0-BAF24E31556C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5CD25D-33FF-471B-9CC9-16CB12533662}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23025" yWindow="2730" windowWidth="15390" windowHeight="9540" xr2:uid="{991B5FBE-8EE9-4B12-9B90-334DFF8DD130}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="15390" windowHeight="9532" xr2:uid="{991B5FBE-8EE9-4B12-9B90-334DFF8DD130}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>PO Number</t>
   </si>
@@ -73,6 +73,135 @@
   </si>
   <si>
     <t>Metrotex Designs</t>
+  </si>
+  <si>
+    <t>CS179233521</t>
+  </si>
+  <si>
+    <t>Pamela Wielander</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (69-4154) X 1, (69-4154) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $53.50 X 1, $53.50 X 1</t>
+  </si>
+  <si>
+    <t>CS179361582</t>
+  </si>
+  <si>
+    <t>Candyce Skimin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (13393) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $15.00 X 1</t>
+  </si>
+  <si>
+    <t>CS179211673</t>
+  </si>
+  <si>
+    <t>Amy Simpkins</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (22009) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $54.00 X 1</t>
+  </si>
+  <si>
+    <t>CA179215641</t>
+  </si>
+  <si>
+    <t>Catherine Dews</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (10263) X 1</t>
+  </si>
+  <si>
+    <t>CS179355305</t>
+  </si>
+  <si>
+    <t>Dr. Cladie Spears</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (28074) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $12.00 X 1</t>
+  </si>
+  <si>
+    <t>CS179295139</t>
+  </si>
+  <si>
+    <t>Nino Putkaradze</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (79-0700) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $6.00 X 1</t>
+  </si>
+  <si>
+    <t>CS179117622</t>
+  </si>
+  <si>
+    <t>Lucy Ferch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (10402) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $195.00 X 1</t>
+  </si>
+  <si>
+    <t>CS179367438</t>
+  </si>
+  <si>
+    <t>Rachelle Locey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (20200) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $140.25 X 1</t>
+  </si>
+  <si>
+    <t>CS179047096</t>
+  </si>
+  <si>
+    <t>Andrea Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (10012) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $14.00 X 1</t>
+  </si>
+  <si>
+    <t>CS179373628</t>
+  </si>
+  <si>
+    <t>Alice Gwinn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (10312) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $32.00 X 1</t>
+  </si>
+  <si>
+    <t>CS179368901</t>
+  </si>
+  <si>
+    <t>Miao Chun Lin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (10329) X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> $75.00 X 1</t>
   </si>
 </sst>
 </file>
@@ -429,23 +558,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914AD4AD-FDB5-4F9E-9466-DB444450799F}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -488,7 +617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -509,6 +638,292 @@
       </c>
       <c r="H3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43689</v>
+      </c>
+      <c r="E4" s="2">
+        <v>107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43690</v>
+      </c>
+      <c r="E5" s="2">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>43689</v>
+      </c>
+      <c r="E6" s="2">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43689</v>
+      </c>
+      <c r="E7" s="2">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43690</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>43690</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43689</v>
+      </c>
+      <c r="E10" s="2">
+        <v>195</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43690</v>
+      </c>
+      <c r="E11" s="2">
+        <v>140.25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43688</v>
+      </c>
+      <c r="E12" s="2">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43690</v>
+      </c>
+      <c r="E13" s="2">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43690</v>
+      </c>
+      <c r="E14" s="2">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>